<commit_message>
data cleanup - player_per_game_df
</commit_message>
<xml_diff>
--- a/aba_mvp_winners.xlsx
+++ b/aba_mvp_winners.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="90">
   <si>
     <t>year_x</t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t>ABA</t>
+  </si>
+  <si>
+    <t>N/A - Stat tracked as of the 1973-74 ABA Season</t>
   </si>
   <si>
     <t>Yes</t>
@@ -939,10 +942,10 @@
         <v>74</v>
       </c>
       <c r="AW2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AX2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:50">
@@ -1088,10 +1091,10 @@
         <v>75</v>
       </c>
       <c r="AW3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AX3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:50">
@@ -1237,10 +1240,10 @@
         <v>75</v>
       </c>
       <c r="AW4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AX4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:50">
@@ -1386,10 +1389,10 @@
         <v>76</v>
       </c>
       <c r="AW5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AX5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:50">
@@ -1516,8 +1519,11 @@
       <c r="AP6">
         <v>6.3</v>
       </c>
-      <c r="AQ6">
-        <v>2.6</v>
+      <c r="AQ6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>87</v>
       </c>
       <c r="AS6">
         <v>4.5</v>
@@ -1532,10 +1538,10 @@
         <v>77</v>
       </c>
       <c r="AW6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AX6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:50">
@@ -1662,8 +1668,11 @@
       <c r="AP7">
         <v>2.7</v>
       </c>
-      <c r="AR7">
-        <v>5</v>
+      <c r="AQ7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>87</v>
       </c>
       <c r="AS7">
         <v>4</v>
@@ -1678,10 +1687,10 @@
         <v>78</v>
       </c>
       <c r="AW7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AX7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:50">
@@ -1808,6 +1817,12 @@
       <c r="AP8">
         <v>2.2</v>
       </c>
+      <c r="AQ8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>87</v>
+      </c>
       <c r="AS8">
         <v>2.8</v>
       </c>
@@ -1821,10 +1836,10 @@
         <v>79</v>
       </c>
       <c r="AW8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AX8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:50">
@@ -1951,6 +1966,12 @@
       <c r="AP9">
         <v>2.3</v>
       </c>
+      <c r="AQ9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>87</v>
+      </c>
       <c r="AS9">
         <v>3</v>
       </c>
@@ -1964,10 +1985,10 @@
         <v>80</v>
       </c>
       <c r="AW9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AX9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:50">
@@ -2094,6 +2115,12 @@
       <c r="AP10">
         <v>1.5</v>
       </c>
+      <c r="AQ10" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>87</v>
+      </c>
       <c r="AS10">
         <v>3.6</v>
       </c>
@@ -2107,10 +2134,10 @@
         <v>81</v>
       </c>
       <c r="AW10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AX10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:50">
@@ -2237,6 +2264,12 @@
       <c r="AP11">
         <v>4.6</v>
       </c>
+      <c r="AQ11" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>87</v>
+      </c>
       <c r="AS11">
         <v>2.9</v>
       </c>
@@ -2250,10 +2283,10 @@
         <v>82</v>
       </c>
       <c r="AW11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AX11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various updates implemented to various dataframes, including calculations
</commit_message>
<xml_diff>
--- a/aba_mvp_winners.xlsx
+++ b/aba_mvp_winners.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="90">
-  <si>
-    <t>year_x</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="91">
+  <si>
+    <t>season_ending_year_x</t>
   </si>
   <si>
     <t>award</t>
@@ -58,7 +58,7 @@
     <t>seas_id_y</t>
   </si>
   <si>
-    <t>year_y</t>
+    <t>season_ending_year_y</t>
   </si>
   <si>
     <t>player_y</t>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>triple_double_avg</t>
+  </si>
+  <si>
+    <t>calendar_year</t>
   </si>
   <si>
     <t>1976</t>
@@ -641,13 +644,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AX11"/>
+  <dimension ref="A1:AY11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:50">
+    <row r="1" spans="1:51">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -798,22 +801,25 @@
       <c r="AX1" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="AY1" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="2" spans="1:50">
+    <row r="2" spans="1:51">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D2">
         <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F2">
         <v>32</v>
@@ -828,7 +834,7 @@
         <v>0.914</v>
       </c>
       <c r="J2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K2">
         <v>6727</v>
@@ -837,22 +843,22 @@
         <v>1381</v>
       </c>
       <c r="M2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N2">
         <v>6727</v>
       </c>
       <c r="O2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="P2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q2">
-        <v>1950</v>
+        <v>1951</v>
       </c>
       <c r="R2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="S2">
         <v>25</v>
@@ -861,10 +867,10 @@
         <v>5</v>
       </c>
       <c r="U2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="W2">
         <v>84</v>
@@ -939,30 +945,33 @@
         <v>29.3</v>
       </c>
       <c r="AV2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AW2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AX2" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="AY2">
+        <v>1976</v>
       </c>
     </row>
-    <row r="3" spans="1:50">
+    <row r="3" spans="1:51">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D3">
         <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F3">
         <v>11</v>
@@ -977,7 +986,7 @@
         <v>0.367</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K3">
         <v>6301</v>
@@ -986,22 +995,22 @@
         <v>1381</v>
       </c>
       <c r="M3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N3">
         <v>6301</v>
       </c>
       <c r="O3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q3">
-        <v>1950</v>
+        <v>1951</v>
       </c>
       <c r="R3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="S3">
         <v>24</v>
@@ -1010,10 +1019,10 @@
         <v>4</v>
       </c>
       <c r="U3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="W3">
         <v>84</v>
@@ -1088,30 +1097,33 @@
         <v>27.9</v>
       </c>
       <c r="AV3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AW3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AX3" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="AY3">
+        <v>1975</v>
       </c>
     </row>
-    <row r="4" spans="1:50">
+    <row r="4" spans="1:51">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D4">
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F4">
         <v>11</v>
@@ -1126,7 +1138,7 @@
         <v>0.367</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K4">
         <v>6220</v>
@@ -1135,22 +1147,22 @@
         <v>1362</v>
       </c>
       <c r="M4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N4">
         <v>6220</v>
       </c>
       <c r="O4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q4">
-        <v>1950</v>
+        <v>1951</v>
       </c>
       <c r="R4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="S4">
         <v>24</v>
@@ -1159,10 +1171,10 @@
         <v>4</v>
       </c>
       <c r="U4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="W4">
         <v>79</v>
@@ -1237,30 +1249,33 @@
         <v>29.8</v>
       </c>
       <c r="AV4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AW4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AX4" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="AY4">
+        <v>1975</v>
       </c>
     </row>
-    <row r="5" spans="1:50">
+    <row r="5" spans="1:51">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5">
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F5">
         <v>49</v>
@@ -1275,7 +1290,7 @@
         <v>0.742</v>
       </c>
       <c r="J5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K5">
         <v>5879</v>
@@ -1284,22 +1299,22 @@
         <v>1381</v>
       </c>
       <c r="M5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N5">
         <v>5879</v>
       </c>
       <c r="O5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q5">
-        <v>1950</v>
+        <v>1951</v>
       </c>
       <c r="R5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="S5">
         <v>23</v>
@@ -1308,10 +1323,10 @@
         <v>3</v>
       </c>
       <c r="U5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="W5">
         <v>84</v>
@@ -1386,30 +1401,33 @@
         <v>27.4</v>
       </c>
       <c r="AV5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AW5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AX5" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="AY5">
+        <v>1974</v>
       </c>
     </row>
-    <row r="6" spans="1:50">
+    <row r="6" spans="1:51">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F6">
         <v>44</v>
@@ -1424,7 +1442,7 @@
         <v>0.759</v>
       </c>
       <c r="J6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K6">
         <v>5247</v>
@@ -1433,22 +1451,22 @@
         <v>842</v>
       </c>
       <c r="M6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N6">
         <v>5247</v>
       </c>
       <c r="O6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Q6">
-        <v>1943</v>
+        <v>1944</v>
       </c>
       <c r="R6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="S6">
         <v>29</v>
@@ -1457,10 +1475,10 @@
         <v>8</v>
       </c>
       <c r="U6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="W6">
         <v>84</v>
@@ -1520,10 +1538,10 @@
         <v>6.3</v>
       </c>
       <c r="AQ6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AR6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AS6">
         <v>4.5</v>
@@ -1535,30 +1553,33 @@
         <v>24.1</v>
       </c>
       <c r="AV6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AW6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AX6" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="AY6">
+        <v>1973</v>
       </c>
     </row>
-    <row r="7" spans="1:50">
+    <row r="7" spans="1:51">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D7">
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F7">
         <v>30</v>
@@ -1573,7 +1594,7 @@
         <v>0.698</v>
       </c>
       <c r="J7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K7">
         <v>4770</v>
@@ -1582,22 +1603,22 @@
         <v>1338</v>
       </c>
       <c r="M7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N7">
         <v>4770</v>
       </c>
       <c r="O7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="P7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="Q7">
-        <v>1949</v>
+        <v>1950</v>
       </c>
       <c r="R7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S7">
         <v>22</v>
@@ -1606,10 +1627,10 @@
         <v>1</v>
       </c>
       <c r="U7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="W7">
         <v>84</v>
@@ -1669,10 +1690,10 @@
         <v>2.7</v>
       </c>
       <c r="AQ7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AR7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AS7">
         <v>4</v>
@@ -1684,30 +1705,33 @@
         <v>23.8</v>
       </c>
       <c r="AV7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AW7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AX7" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="AY7">
+        <v>1972</v>
       </c>
     </row>
-    <row r="8" spans="1:50">
+    <row r="8" spans="1:51">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D8">
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F8">
         <v>9</v>
@@ -1722,7 +1746,7 @@
         <v>0.764</v>
       </c>
       <c r="J8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K8">
         <v>4631</v>
@@ -1731,22 +1755,22 @@
         <v>1013</v>
       </c>
       <c r="M8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N8">
         <v>4631</v>
       </c>
       <c r="O8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Q8">
-        <v>1944</v>
+        <v>1945</v>
       </c>
       <c r="R8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S8">
         <v>26</v>
@@ -1755,10 +1779,10 @@
         <v>4</v>
       </c>
       <c r="U8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="W8">
         <v>82</v>
@@ -1818,10 +1842,10 @@
         <v>2.2</v>
       </c>
       <c r="AQ8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AR8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AS8">
         <v>2.8</v>
@@ -1833,30 +1857,33 @@
         <v>21</v>
       </c>
       <c r="AV8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AW8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AX8" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="AY8">
+        <v>1971</v>
       </c>
     </row>
-    <row r="9" spans="1:50">
+    <row r="9" spans="1:51">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D9">
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F9">
         <v>17</v>
@@ -1871,7 +1898,7 @@
         <v>0.97</v>
       </c>
       <c r="J9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K9">
         <v>4254</v>
@@ -1880,22 +1907,22 @@
         <v>1226</v>
       </c>
       <c r="M9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N9">
         <v>4254</v>
       </c>
       <c r="O9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="P9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q9">
-        <v>1949</v>
+        <v>1950</v>
       </c>
       <c r="R9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S9">
         <v>20</v>
@@ -1904,10 +1931,10 @@
         <v>1</v>
       </c>
       <c r="U9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="W9">
         <v>84</v>
@@ -1967,10 +1994,10 @@
         <v>2.3</v>
       </c>
       <c r="AQ9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AR9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AS9">
         <v>3</v>
@@ -1982,30 +2009,33 @@
         <v>30</v>
       </c>
       <c r="AV9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AW9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AX9" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="AY9">
+        <v>1970</v>
       </c>
     </row>
-    <row r="10" spans="1:50">
+    <row r="10" spans="1:51">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D10">
         <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F10">
         <v>8</v>
@@ -2020,7 +2050,7 @@
         <v>0.909</v>
       </c>
       <c r="J10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K10">
         <v>3771</v>
@@ -2029,22 +2059,22 @@
         <v>1013</v>
       </c>
       <c r="M10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N10">
         <v>3771</v>
       </c>
       <c r="O10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="P10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Q10">
-        <v>1944</v>
+        <v>1945</v>
       </c>
       <c r="R10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S10">
         <v>24</v>
@@ -2053,10 +2083,10 @@
         <v>2</v>
       </c>
       <c r="U10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="W10">
         <v>76</v>
@@ -2116,10 +2146,10 @@
         <v>1.5</v>
       </c>
       <c r="AQ10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AR10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AS10">
         <v>3.6</v>
@@ -2131,30 +2161,33 @@
         <v>24</v>
       </c>
       <c r="AV10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AW10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AX10" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="AY10">
+        <v>1969</v>
       </c>
     </row>
-    <row r="11" spans="1:50">
+    <row r="11" spans="1:51">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D11">
         <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F11">
         <v>19</v>
@@ -2169,7 +2202,7 @@
         <v>0.983</v>
       </c>
       <c r="J11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K11">
         <v>3189</v>
@@ -2178,22 +2211,22 @@
         <v>934</v>
       </c>
       <c r="M11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N11">
         <v>3189</v>
       </c>
       <c r="O11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q11">
-        <v>1942</v>
+        <v>1943</v>
       </c>
       <c r="R11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S11">
         <v>25</v>
@@ -2202,10 +2235,10 @@
         <v>1</v>
       </c>
       <c r="U11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W11">
         <v>70</v>
@@ -2265,10 +2298,10 @@
         <v>4.6</v>
       </c>
       <c r="AQ11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AR11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AS11">
         <v>2.9</v>
@@ -2280,13 +2313,16 @@
         <v>26.8</v>
       </c>
       <c r="AV11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AW11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AX11" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="AY11">
+        <v>1968</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various updates successfully implemented
</commit_message>
<xml_diff>
--- a/aba_mvp_winners.xlsx
+++ b/aba_mvp_winners.xlsx
@@ -855,13 +855,13 @@
         <v>61</v>
       </c>
       <c r="Q2">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="R2" t="s">
         <v>84</v>
       </c>
       <c r="S2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T2">
         <v>5</v>
@@ -1007,13 +1007,13 @@
         <v>61</v>
       </c>
       <c r="Q3">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="R3" t="s">
         <v>84</v>
       </c>
       <c r="S3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T3">
         <v>4</v>
@@ -1159,13 +1159,13 @@
         <v>62</v>
       </c>
       <c r="Q4">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="R4" t="s">
         <v>85</v>
       </c>
       <c r="S4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T4">
         <v>4</v>
@@ -1311,13 +1311,13 @@
         <v>61</v>
       </c>
       <c r="Q5">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="R5" t="s">
         <v>84</v>
       </c>
       <c r="S5">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T5">
         <v>3</v>
@@ -1463,13 +1463,13 @@
         <v>63</v>
       </c>
       <c r="Q6">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="R6" t="s">
         <v>85</v>
       </c>
       <c r="S6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="T6">
         <v>8</v>
@@ -1615,13 +1615,13 @@
         <v>64</v>
       </c>
       <c r="Q7">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="R7" t="s">
         <v>86</v>
       </c>
       <c r="S7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T7">
         <v>1</v>
@@ -1767,13 +1767,13 @@
         <v>65</v>
       </c>
       <c r="Q8">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="R8" t="s">
         <v>86</v>
       </c>
       <c r="S8">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T8">
         <v>4</v>
@@ -1919,13 +1919,13 @@
         <v>66</v>
       </c>
       <c r="Q9">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="R9" t="s">
         <v>86</v>
       </c>
       <c r="S9">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="T9">
         <v>1</v>
@@ -2071,13 +2071,13 @@
         <v>65</v>
       </c>
       <c r="Q10">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="R10" t="s">
         <v>86</v>
       </c>
       <c r="S10">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T10">
         <v>2</v>
@@ -2223,13 +2223,13 @@
         <v>67</v>
       </c>
       <c r="Q11">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="R11" t="s">
         <v>86</v>
       </c>
       <c r="S11">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T11">
         <v>1</v>

</xml_diff>

<commit_message>
recreation of merges, pivot tables, charts, and conditional formatting of various dataframes
</commit_message>
<xml_diff>
--- a/aba_mvp_winners.xlsx
+++ b/aba_mvp_winners.xlsx
@@ -46,19 +46,19 @@
     <t>winner</t>
   </si>
   <si>
-    <t>seas_id_x</t>
-  </si>
-  <si>
-    <t>player_id</t>
+    <t>seas_id</t>
+  </si>
+  <si>
+    <t>player_id_x</t>
   </si>
   <si>
     <t>season_x</t>
   </si>
   <si>
-    <t>seas_id_y</t>
-  </si>
-  <si>
     <t>season_ending_year_y</t>
+  </si>
+  <si>
+    <t>player_id_y</t>
   </si>
   <si>
     <t>player_y</t>
@@ -845,11 +845,11 @@
       <c r="M2" t="s">
         <v>75</v>
       </c>
-      <c r="N2">
-        <v>6727</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="N2" t="s">
         <v>51</v>
+      </c>
+      <c r="O2">
+        <v>2932</v>
       </c>
       <c r="P2" t="s">
         <v>61</v>
@@ -997,11 +997,11 @@
       <c r="M3" t="s">
         <v>76</v>
       </c>
-      <c r="N3">
-        <v>6301</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="N3" t="s">
         <v>52</v>
+      </c>
+      <c r="O3">
+        <v>2932</v>
       </c>
       <c r="P3" t="s">
         <v>61</v>
@@ -1149,11 +1149,11 @@
       <c r="M4" t="s">
         <v>76</v>
       </c>
-      <c r="N4">
-        <v>6220</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="N4" t="s">
         <v>52</v>
+      </c>
+      <c r="O4">
+        <v>1906</v>
       </c>
       <c r="P4" t="s">
         <v>62</v>
@@ -1301,11 +1301,11 @@
       <c r="M5" t="s">
         <v>77</v>
       </c>
-      <c r="N5">
-        <v>5879</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="N5" t="s">
         <v>53</v>
+      </c>
+      <c r="O5">
+        <v>2932</v>
       </c>
       <c r="P5" t="s">
         <v>61</v>
@@ -1453,11 +1453,11 @@
       <c r="M6" t="s">
         <v>78</v>
       </c>
-      <c r="N6">
-        <v>5247</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="N6" t="s">
         <v>54</v>
+      </c>
+      <c r="O6">
+        <v>426</v>
       </c>
       <c r="P6" t="s">
         <v>63</v>
@@ -1605,11 +1605,11 @@
       <c r="M7" t="s">
         <v>79</v>
       </c>
-      <c r="N7">
-        <v>4770</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="N7" t="s">
         <v>55</v>
+      </c>
+      <c r="O7">
+        <v>293</v>
       </c>
       <c r="P7" t="s">
         <v>64</v>
@@ -1757,11 +1757,11 @@
       <c r="M8" t="s">
         <v>80</v>
       </c>
-      <c r="N8">
-        <v>4631</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="N8" t="s">
         <v>56</v>
+      </c>
+      <c r="O8">
+        <v>3599</v>
       </c>
       <c r="P8" t="s">
         <v>65</v>
@@ -1909,11 +1909,11 @@
       <c r="M9" t="s">
         <v>81</v>
       </c>
-      <c r="N9">
-        <v>4254</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="N9" t="s">
         <v>57</v>
+      </c>
+      <c r="O9">
+        <v>4639</v>
       </c>
       <c r="P9" t="s">
         <v>66</v>
@@ -2061,11 +2061,11 @@
       <c r="M10" t="s">
         <v>82</v>
       </c>
-      <c r="N10">
-        <v>3771</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="N10" t="s">
         <v>58</v>
+      </c>
+      <c r="O10">
+        <v>3599</v>
       </c>
       <c r="P10" t="s">
         <v>65</v>
@@ -2213,11 +2213,11 @@
       <c r="M11" t="s">
         <v>83</v>
       </c>
-      <c r="N11">
-        <v>3189</v>
-      </c>
-      <c r="O11" t="s">
+      <c r="N11" t="s">
         <v>59</v>
+      </c>
+      <c r="O11">
+        <v>1008</v>
       </c>
       <c r="P11" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
downloaded updated csvs from kaggle.com
</commit_message>
<xml_diff>
--- a/aba_mvp_winners.xlsx
+++ b/aba_mvp_winners.xlsx
@@ -849,7 +849,7 @@
         <v>51</v>
       </c>
       <c r="O2">
-        <v>2932</v>
+        <v>2937</v>
       </c>
       <c r="P2" t="s">
         <v>61</v>
@@ -1001,7 +1001,7 @@
         <v>52</v>
       </c>
       <c r="O3">
-        <v>2932</v>
+        <v>2937</v>
       </c>
       <c r="P3" t="s">
         <v>61</v>
@@ -1153,7 +1153,7 @@
         <v>52</v>
       </c>
       <c r="O4">
-        <v>1906</v>
+        <v>1910</v>
       </c>
       <c r="P4" t="s">
         <v>62</v>
@@ -1305,7 +1305,7 @@
         <v>53</v>
       </c>
       <c r="O5">
-        <v>2932</v>
+        <v>2937</v>
       </c>
       <c r="P5" t="s">
         <v>61</v>
@@ -1761,7 +1761,7 @@
         <v>56</v>
       </c>
       <c r="O8">
-        <v>3599</v>
+        <v>3605</v>
       </c>
       <c r="P8" t="s">
         <v>65</v>
@@ -1913,7 +1913,7 @@
         <v>57</v>
       </c>
       <c r="O9">
-        <v>4639</v>
+        <v>4646</v>
       </c>
       <c r="P9" t="s">
         <v>66</v>
@@ -2065,7 +2065,7 @@
         <v>58</v>
       </c>
       <c r="O10">
-        <v>3599</v>
+        <v>3605</v>
       </c>
       <c r="P10" t="s">
         <v>65</v>
@@ -2217,7 +2217,7 @@
         <v>59</v>
       </c>
       <c r="O11">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="P11" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
code added patrick ewing and hakeem olajuwon per game avgs dataframes; more dataframes to be developed based on the careers of the aformentioned players
</commit_message>
<xml_diff>
--- a/aba_mvp_winners.xlsx
+++ b/aba_mvp_winners.xlsx
@@ -1150,7 +1150,7 @@
         <v>52</v>
       </c>
       <c r="O4">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="P4" t="s">
         <v>62</v>
@@ -1454,7 +1454,7 @@
         <v>54</v>
       </c>
       <c r="O6">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="P6" t="s">
         <v>63</v>
@@ -1603,7 +1603,7 @@
         <v>55</v>
       </c>
       <c r="O7">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P7" t="s">
         <v>64</v>
@@ -1752,7 +1752,7 @@
         <v>56</v>
       </c>
       <c r="O8">
-        <v>3605</v>
+        <v>3606</v>
       </c>
       <c r="P8" t="s">
         <v>65</v>
@@ -1898,7 +1898,7 @@
         <v>57</v>
       </c>
       <c r="O9">
-        <v>4646</v>
+        <v>4644</v>
       </c>
       <c r="P9" t="s">
         <v>66</v>
@@ -2044,7 +2044,7 @@
         <v>58</v>
       </c>
       <c r="O10">
-        <v>3605</v>
+        <v>3606</v>
       </c>
       <c r="P10" t="s">
         <v>65</v>
@@ -2190,7 +2190,7 @@
         <v>59</v>
       </c>
       <c r="O11">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="P11" t="s">
         <v>67</v>

</xml_diff>